<commit_message>
test uniformisation des filtres
</commit_message>
<xml_diff>
--- a/bdd/bdd_train.xlsx
+++ b/bdd/bdd_train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elevate\Documents\PowerBI_LLM\PowerBI-LLM\bdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561F149C-897F-44ED-B7E9-0FB55AC36B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316F732E-AD0D-4CB2-AF42-649E168BF621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BEC43D25-63C5-48CA-857E-16019B125449}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>json_path_before_change</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>jsons_train/titre_rapport_it.json</t>
+  </si>
+  <si>
+    <t>Ajoute un xljfsn du nombre distinct de session_id</t>
+  </si>
+  <si>
+    <t>Desole je ne reconnais pas le terme "xljfsn"</t>
+  </si>
+  <si>
+    <t>Ajoute un graphique en etoile des variables de la table</t>
+  </si>
+  <si>
+    <t>Desole mais le visuel "graphique en etoile" n'est pas disponible dans Power BI</t>
   </si>
 </sst>
 </file>
@@ -488,16 +500,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7405241D-8C65-43C0-B6BC-A90E331BB2DA}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7265625" customWidth="1"/>
+    <col min="2" max="2" width="60.90625" customWidth="1"/>
+    <col min="3" max="3" width="82.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -621,6 +634,28 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>